<commit_message>
feat(backend): add Cart entity, NRT and make refactorings
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D02C25C-D988-42D7-B627-E5D6BE1012D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4312A5A2-821F-463A-A2FF-143D5A5A472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>1. hét</t>
   </si>
@@ -78,21 +78,9 @@
     <t>TODO</t>
   </si>
   <si>
-    <t>Feladatkiírás, projekt rendbeszedése</t>
-  </si>
-  <si>
-    <t>Felhasználókezelés</t>
-  </si>
-  <si>
     <t>Admin felület (áruk hozzáadása, törlése, szerkesztése, rendelések nézése)</t>
   </si>
   <si>
-    <t>Shop filters</t>
-  </si>
-  <si>
-    <t>Fizetés</t>
-  </si>
-  <si>
     <t>Android kliens</t>
   </si>
   <si>
@@ -102,10 +90,37 @@
     <t>Ajánló motor, tesztelés, deployment</t>
   </si>
   <si>
-    <t>Üzleti folyamat feltérképezés</t>
-  </si>
-  <si>
-    <t>Kereső optimalizálás</t>
+    <t>Felhasználókezelés - utánaolvasni, hogy hogyan működik - Angular és ASP.NET authentication</t>
+  </si>
+  <si>
+    <t>Felhasználókezelés - felület létrehozás - bejelentkezés, profil, rendeléseim képernyő</t>
+  </si>
+  <si>
+    <t>Shop filters - utánaolvasni, hogyan szokás elkészíteni, backend queryk? Megvalósítása</t>
+  </si>
+  <si>
+    <t>Shop filters - webes kliensben megvalósítás - shopban filter felület, filter service?</t>
+  </si>
+  <si>
+    <t>Fizetés - utánanézni, milyen lehetőségek vannak, hogyan lehet beépíteni őket, ki lehet-e próbálni őket</t>
+  </si>
+  <si>
+    <t>Webes fizetés megvalósítása</t>
+  </si>
+  <si>
+    <t>Kereső optimalizálás - utánanézni, milyen módszerek vannak rá, hogyan érdemes csinálni, implementálni</t>
+  </si>
+  <si>
+    <t>nyár</t>
+  </si>
+  <si>
+    <t>Feladatkiírás, projekt rendbeszedése, ütemterv részletesebb elkészítése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Üzleti folyamat feltérképezés, Felhasználókezelés - backend megvalósítás, frontenden servicek megvalósítása, </t>
+  </si>
+  <si>
+    <t>TODO: Android wireframe</t>
   </si>
 </sst>
 </file>
@@ -163,7 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -441,17 +456,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="98.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,7 +488,7 @@
         <v>44606</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,7 +499,7 @@
         <v>44613</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,7 +510,7 @@
         <v>44620</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,7 +521,7 @@
         <v>44627</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,7 +532,7 @@
         <v>44634</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +543,7 @@
         <v>44641</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -539,7 +554,7 @@
         <v>44648</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,7 +565,7 @@
         <v>44655</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -561,7 +576,7 @@
         <v>44662</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -572,7 +587,7 @@
         <v>44669</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +598,7 @@
         <v>44676</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -594,7 +609,7 @@
         <v>44683</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,7 +620,7 @@
         <v>44690</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,15 +631,28 @@
         <v>44697</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(backend): improve domain models
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4312A5A2-821F-463A-A2FF-143D5A5A472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7CF14A-6650-4520-BA4C-FADDC03BF1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,15 +93,6 @@
     <t>Felhasználókezelés - utánaolvasni, hogy hogyan működik - Angular és ASP.NET authentication</t>
   </si>
   <si>
-    <t>Felhasználókezelés - felület létrehozás - bejelentkezés, profil, rendeléseim képernyő</t>
-  </si>
-  <si>
-    <t>Shop filters - utánaolvasni, hogyan szokás elkészíteni, backend queryk? Megvalósítása</t>
-  </si>
-  <si>
-    <t>Shop filters - webes kliensben megvalósítás - shopban filter felület, filter service?</t>
-  </si>
-  <si>
     <t>Fizetés - utánanézni, milyen lehetőségek vannak, hogyan lehet beépíteni őket, ki lehet-e próbálni őket</t>
   </si>
   <si>
@@ -117,10 +108,19 @@
     <t>Feladatkiírás, projekt rendbeszedése, ütemterv részletesebb elkészítése</t>
   </si>
   <si>
-    <t xml:space="preserve">Üzleti folyamat feltérképezés, Felhasználókezelés - backend megvalósítás, frontenden servicek megvalósítása, </t>
-  </si>
-  <si>
     <t>TODO: Android wireframe</t>
+  </si>
+  <si>
+    <t>Shop filters - utánaolvasni, hogyan szokás elkészíteni, backend queryk? Megvalósítása, webes kliensben megvalósítás - shopban filter felület, filter service?</t>
+  </si>
+  <si>
+    <t>Felhasználókezelés, kosár kezelése - felület létrehozás - bejelentkezés, profil, rendeléseim képernyő</t>
+  </si>
+  <si>
+    <t>Üzleti folyamat feltérképezés, Felhasználókezelés, kosár kezelése, utánanézni, mik a lehetőségek</t>
+  </si>
+  <si>
+    <t>Felhasználókezelés, kosár kezelése - backend megvalósítás, backend - NRT hozzáadása, Domain fejlesztése, refaktorálás</t>
   </si>
 </sst>
 </file>
@@ -459,14 +459,14 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+    <col min="3" max="3" width="138.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
         <v>44606</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -521,7 +521,7 @@
         <v>44627</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>44634</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
         <v>44641</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>44662</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>44669</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,7 +598,7 @@
         <v>44676</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(api): implement RefreshToken based authentication
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7CF14A-6650-4520-BA4C-FADDC03BF1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E848244-6366-4E2C-9FEB-FA752D978455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>1. hét</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>Felhasználókezelés, kosár kezelése - backend megvalósítás, backend - NRT hozzáadása, Domain fejlesztése, refaktorálás</t>
+  </si>
+  <si>
+    <t>csúszás</t>
+  </si>
+  <si>
+    <t>Felhasználókezelés backenden - refresh token megoldása</t>
+  </si>
+  <si>
+    <t>Felhasználókezelés backenden - NRT miatt változtatások</t>
   </si>
 </sst>
 </file>
@@ -456,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +478,7 @@
     <col min="3" max="3" width="138.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -480,7 +489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +500,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -502,7 +511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -513,7 +522,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -524,7 +533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -532,10 +541,13 @@
         <v>44634</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,10 +555,13 @@
         <v>44641</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -554,10 +569,10 @@
         <v>44648</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -565,10 +580,10 @@
         <v>44655</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -576,10 +591,10 @@
         <v>44662</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -587,10 +602,10 @@
         <v>44669</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -598,10 +613,10 @@
         <v>44676</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -609,10 +624,10 @@
         <v>44683</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -620,10 +635,10 @@
         <v>44690</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -634,7 +649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -647,6 +662,16 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(webapp, api): create GetUserOrders, fix login, fix dtos and viewmodels
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E848244-6366-4E2C-9FEB-FA752D978455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFB1FBB-A27B-4C8E-A060-7728C0221144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>1. hét</t>
   </si>
@@ -571,6 +571,9 @@
       <c r="C8" t="s">
         <v>29</v>
       </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">

</xml_diff>

<commit_message>
feat(api, webapp): api controller fixes done, webapp skeleton created
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFB1FBB-A27B-4C8E-A060-7728C0221144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4076B8-5C98-4C71-AE15-E1418A3DBCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>1. hét</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Shop filters - utánaolvasni, hogyan szokás elkészíteni, backend queryk? Megvalósítása, webes kliensben megvalósítás - shopban filter felület, filter service?</t>
   </si>
   <si>
-    <t>Felhasználókezelés, kosár kezelése - felület létrehozás - bejelentkezés, profil, rendeléseim képernyő</t>
-  </si>
-  <si>
     <t>Üzleti folyamat feltérképezés, Felhasználókezelés, kosár kezelése, utánanézni, mik a lehetőségek</t>
   </si>
   <si>
@@ -130,6 +127,24 @@
   </si>
   <si>
     <t>Felhasználókezelés backenden - NRT miatt változtatások</t>
+  </si>
+  <si>
+    <t>Kosár kezelése - CartService megvalósítása</t>
+  </si>
+  <si>
+    <t>Kliens alkalmazás létrehozása, függőségek telepítése, Angular Material téma kialakítása</t>
+  </si>
+  <si>
+    <t>Felhasználókezelés, kosár kezelése - felület létrehozás - bejelentkezés, profil, rendeléseim képernyő (tipikus user flow)</t>
+  </si>
+  <si>
+    <t>Kliens alkalmazás basic layout, Felhasználókezelés - refresh token autentikáció</t>
+  </si>
+  <si>
+    <t>RxJS betanulás - Subject, BehaviorSubject, Operators (pipe, map, tap, switchMap...), Kliens alkalmazás reszponzív header</t>
+  </si>
+  <si>
+    <t>Dokumentáció írás (technológiák bemutatása, végleges részek bemutatása)</t>
   </si>
 </sst>
 </file>
@@ -465,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +491,7 @@
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="138.7109375" customWidth="1"/>
+    <col min="4" max="4" width="77.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -519,7 +535,7 @@
         <v>44620</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,7 +546,7 @@
         <v>44627</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,10 +557,10 @@
         <v>44634</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,10 +571,10 @@
         <v>44641</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,10 +585,10 @@
         <v>44648</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,7 +599,7 @@
         <v>44655</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,7 +610,7 @@
         <v>44662</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -605,7 +621,7 @@
         <v>44669</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,7 +632,7 @@
         <v>44676</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +643,7 @@
         <v>44683</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,7 +654,7 @@
         <v>44690</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,7 +665,10 @@
         <v>44697</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -657,7 +676,7 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,22 +684,45 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(webapp): product filter work
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4076B8-5C98-4C71-AE15-E1418A3DBCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A957057-1381-4BE5-B85D-663490A22A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>1. hét</t>
   </si>
@@ -78,80 +78,59 @@
     <t>TODO</t>
   </si>
   <si>
-    <t>Admin felület (áruk hozzáadása, törlése, szerkesztése, rendelések nézése)</t>
-  </si>
-  <si>
-    <t>Android kliens</t>
-  </si>
-  <si>
-    <t>2. félév:</t>
-  </si>
-  <si>
-    <t>Ajánló motor, tesztelés, deployment</t>
-  </si>
-  <si>
-    <t>Felhasználókezelés - utánaolvasni, hogy hogyan működik - Angular és ASP.NET authentication</t>
-  </si>
-  <si>
-    <t>Fizetés - utánanézni, milyen lehetőségek vannak, hogyan lehet beépíteni őket, ki lehet-e próbálni őket</t>
-  </si>
-  <si>
-    <t>Webes fizetés megvalósítása</t>
-  </si>
-  <si>
-    <t>Kereső optimalizálás - utánanézni, milyen módszerek vannak rá, hogyan érdemes csinálni, implementálni</t>
-  </si>
-  <si>
-    <t>nyár</t>
-  </si>
-  <si>
-    <t>Feladatkiírás, projekt rendbeszedése, ütemterv részletesebb elkészítése</t>
-  </si>
-  <si>
-    <t>TODO: Android wireframe</t>
-  </si>
-  <si>
-    <t>Shop filters - utánaolvasni, hogyan szokás elkészíteni, backend queryk? Megvalósítása, webes kliensben megvalósítás - shopban filter felület, filter service?</t>
-  </si>
-  <si>
-    <t>Üzleti folyamat feltérképezés, Felhasználókezelés, kosár kezelése, utánanézni, mik a lehetőségek</t>
-  </si>
-  <si>
-    <t>Felhasználókezelés, kosár kezelése - backend megvalósítás, backend - NRT hozzáadása, Domain fejlesztése, refaktorálás</t>
-  </si>
-  <si>
-    <t>csúszás</t>
-  </si>
-  <si>
-    <t>Felhasználókezelés backenden - refresh token megoldása</t>
-  </si>
-  <si>
-    <t>Felhasználókezelés backenden - NRT miatt változtatások</t>
-  </si>
-  <si>
-    <t>Kosár kezelése - CartService megvalósítása</t>
-  </si>
-  <si>
-    <t>Kliens alkalmazás létrehozása, függőségek telepítése, Angular Material téma kialakítása</t>
-  </si>
-  <si>
-    <t>Felhasználókezelés, kosár kezelése - felület létrehozás - bejelentkezés, profil, rendeléseim képernyő (tipikus user flow)</t>
-  </si>
-  <si>
-    <t>Kliens alkalmazás basic layout, Felhasználókezelés - refresh token autentikáció</t>
-  </si>
-  <si>
-    <t>RxJS betanulás - Subject, BehaviorSubject, Operators (pipe, map, tap, switchMap...), Kliens alkalmazás reszponzív header</t>
-  </si>
-  <si>
-    <t>Dokumentáció írás (technológiák bemutatása, végleges részek bemutatása)</t>
+    <t>Termék filterezés</t>
+  </si>
+  <si>
+    <t>Termék filterezés, webes fizetés</t>
+  </si>
+  <si>
+    <t>Android kliens - architektura megtervezés, app skeleton létrehozása</t>
+  </si>
+  <si>
+    <t>Android kliens - kezdőképernyő, autentikáció megvalósítás, lokális adatbázis megvalósítás</t>
+  </si>
+  <si>
+    <t>Android kliens - termékek, kosár, checkout képernyők megvalósítása</t>
+  </si>
+  <si>
+    <t>Android kliens - termék filterezés megvalósítása</t>
+  </si>
+  <si>
+    <t>Diplomamunka írás</t>
+  </si>
+  <si>
+    <t>Beadási határidő</t>
+  </si>
+  <si>
+    <t>2022.12.09, 12 óra</t>
+  </si>
+  <si>
+    <t>Nyáron elkészült:</t>
+  </si>
+  <si>
+    <t>Webes fizetés, tesztek készítése</t>
+  </si>
+  <si>
+    <t>backend és fronted pagination rendelésekhez (admin) és termékekhez (user)</t>
+  </si>
+  <si>
+    <t>színek, anyagok, minták kezelése</t>
+  </si>
+  <si>
+    <t>rendelések és termékek query-zése (filterezés, rendezés)</t>
+  </si>
+  <si>
+    <t>teljes admin felület (rendelések megtekintése, termékeken, kategóriákon CRUD műveletek)</t>
+  </si>
+  <si>
+    <t>termékek és kategóriák képeinek kezelése - backenden külön thumbnail és original lementése (3rd party könyvtár segítségével)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +149,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,11 +181,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -480,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +481,7 @@
     <col min="4" max="4" width="77.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -505,224 +492,198 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44606</v>
+        <v>44809</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>44613</v>
+        <v>44816</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>44620</v>
+        <v>44823</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>44627</v>
+        <v>44830</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>44634</v>
+        <v>44837</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>44641</v>
+        <v>44844</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>44648</v>
+        <v>44851</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>44655</v>
+        <v>44858</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>44662</v>
+        <v>44865</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>44669</v>
+        <v>44872</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>44676</v>
+        <v>44879</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>44683</v>
+        <v>44886</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>44690</v>
+        <v>44893</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>44697</v>
+        <v>44900</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(webapp): UI improvements, schedule modified
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A957057-1381-4BE5-B85D-663490A22A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98F3718-20F1-494C-AE87-21AE17D911FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>1. hét</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Termék filterezés</t>
   </si>
   <si>
-    <t>Termék filterezés, webes fizetés</t>
-  </si>
-  <si>
     <t>Android kliens - architektura megtervezés, app skeleton létrehozása</t>
   </si>
   <si>
@@ -124,6 +121,15 @@
   </si>
   <si>
     <t>termékek és kategóriák képeinek kezelése - backenden külön thumbnail és original lementése (3rd party könyvtár segítségével)</t>
+  </si>
+  <si>
+    <t>Termék filterezés, landing page, UI szépítése</t>
+  </si>
+  <si>
+    <t>Deployment, hosting, webes fizetés</t>
+  </si>
+  <si>
+    <t>Deployment, hosting, webes fizetés, tesztek készítése</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +517,7 @@
         <v>44816</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -522,7 +528,7 @@
         <v>44823</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,7 +539,7 @@
         <v>44830</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,7 +550,7 @@
         <v>44837</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,7 +561,7 @@
         <v>44844</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -566,7 +572,7 @@
         <v>44851</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -577,7 +583,7 @@
         <v>44858</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,7 +594,7 @@
         <v>44865</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,7 +605,7 @@
         <v>44872</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -610,7 +616,7 @@
         <v>44879</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,7 +627,7 @@
         <v>44886</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,7 +638,7 @@
         <v>44893</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,15 +649,15 @@
         <v>44900</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,31 +665,31 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(webapp, webapi): fixes for webpayment
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98F3718-20F1-494C-AE87-21AE17D911FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED44057-D40E-4E9C-9B8E-D4D92A37DB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>1. hét</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Termék filterezés</t>
   </si>
   <si>
-    <t>Android kliens - architektura megtervezés, app skeleton létrehozása</t>
-  </si>
-  <si>
     <t>Android kliens - kezdőképernyő, autentikáció megvalósítás, lokális adatbázis megvalósítás</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Nyáron elkészült:</t>
   </si>
   <si>
-    <t>Webes fizetés, tesztek készítése</t>
-  </si>
-  <si>
     <t>backend és fronted pagination rendelésekhez (admin) és termékekhez (user)</t>
   </si>
   <si>
@@ -129,7 +123,10 @@
     <t>Deployment, hosting, webes fizetés</t>
   </si>
   <si>
-    <t>Deployment, hosting, webes fizetés, tesztek készítése</t>
+    <t>Webes fizetés</t>
+  </si>
+  <si>
+    <t>Webes fizetés production-ben, Tesztek készítése, Android kliens - architektura megtervezés, app skeleton létrehozása</t>
   </si>
 </sst>
 </file>
@@ -476,7 +473,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +514,7 @@
         <v>44816</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +525,7 @@
         <v>44823</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -539,7 +536,7 @@
         <v>44830</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,7 +547,7 @@
         <v>44837</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -561,7 +558,7 @@
         <v>44844</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -572,7 +569,7 @@
         <v>44851</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +580,7 @@
         <v>44858</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -594,7 +591,7 @@
         <v>44865</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,7 +602,7 @@
         <v>44872</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,7 +613,7 @@
         <v>44879</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +624,7 @@
         <v>44886</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,7 +635,7 @@
         <v>44893</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,15 +646,15 @@
         <v>44900</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,31 +662,31 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(android): create screens and bottom nav
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED44057-D40E-4E9C-9B8E-D4D92A37DB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C702D5-7EA4-4F39-AB86-8008413CAA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,12 +84,6 @@
     <t>Android kliens - kezdőképernyő, autentikáció megvalósítás, lokális adatbázis megvalósítás</t>
   </si>
   <si>
-    <t>Android kliens - termékek, kosár, checkout képernyők megvalósítása</t>
-  </si>
-  <si>
-    <t>Android kliens - termék filterezés megvalósítása</t>
-  </si>
-  <si>
     <t>Diplomamunka írás</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>Webes fizetés production-ben, Tesztek készítése, Android kliens - architektura megtervezés, app skeleton létrehozása</t>
+  </si>
+  <si>
+    <t>Android Compose betanulás</t>
+  </si>
+  <si>
+    <t>Android kliens - termékek, kosár, checkout képernyők megvalósítása,  termék filterezés megvalósítása</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
         <v>44816</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>44823</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>44830</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>44837</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>44844</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>44851</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>44858</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
         <v>44865</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>44872</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>44879</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>44886</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>44893</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,15 +646,15 @@
         <v>44900</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,31 +662,31 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(android): product category work
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\CurlyCircle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C702D5-7EA4-4F39-AB86-8008413CAA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97447529-649F-4701-8044-784B320E6E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>1. hét</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Termék filterezés</t>
   </si>
   <si>
-    <t>Android kliens - kezdőképernyő, autentikáció megvalósítás, lokális adatbázis megvalósítás</t>
-  </si>
-  <si>
     <t>Diplomamunka írás</t>
   </si>
   <si>
@@ -123,10 +120,19 @@
     <t>Webes fizetés production-ben, Tesztek készítése, Android kliens - architektura megtervezés, app skeleton létrehozása</t>
   </si>
   <si>
-    <t>Android Compose betanulás</t>
-  </si>
-  <si>
-    <t>Android kliens - termékek, kosár, checkout képernyők megvalósítása,  termék filterezés megvalósítása</t>
+    <t xml:space="preserve">Android Compose betanulás </t>
+  </si>
+  <si>
+    <t>Android kliens -  kosár, checkout képernyők megvalósítása,  termék filterezés megvalósítása - Diplomamunka írás</t>
+  </si>
+  <si>
+    <t>Android kliens - termékek, termékkategóriák, autentikáció megvalósítás, lokális adatbázis megvalósítás</t>
+  </si>
+  <si>
+    <t>Android kliens - architektura, app skeleton kialakítása, technológiák kiválasztása, függőségek hozzáadása, navigáció megvalósítása</t>
+  </si>
+  <si>
+    <t>Android Architecture, Navigation betanulás</t>
   </si>
 </sst>
 </file>
@@ -473,7 +479,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +520,7 @@
         <v>44816</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,7 +531,7 @@
         <v>44823</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,7 +542,7 @@
         <v>44830</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +553,7 @@
         <v>44837</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,7 +564,7 @@
         <v>44844</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,7 +575,7 @@
         <v>44851</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +586,7 @@
         <v>44858</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,7 +597,7 @@
         <v>44865</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +608,7 @@
         <v>44872</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,7 +619,7 @@
         <v>44879</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,7 +630,7 @@
         <v>44886</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +641,7 @@
         <v>44893</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,15 +652,15 @@
         <v>44900</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,31 +668,31 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>